<commit_message>
Nuuchahnulth: update data progress
</commit_message>
<xml_diff>
--- a/resources/Nuuchahnulth data progress.xlsx
+++ b/resources/Nuuchahnulth data progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwhie\OneDrive\Dissertation\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="531" documentId="8_{F2A7D79F-8BBB-41F1-8705-2F7625968273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA74C84F-55DB-4C5E-8ABA-94C60B107343}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A3B152-C5C7-4356-9DA1-36E6564494A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{6896C122-56FA-4CA3-9120-A32E86371320}"/>
   </bookViews>
@@ -315,7 +315,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.13975903614457832</c:v>
+                  <c:v>0.17309236947791165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,6 +994,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.8602409638554217</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82690763052208838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2704,7 +2707,7 @@
   <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2775,7 +2778,7 @@
       </c>
       <c r="D6" s="4">
         <f>MAX(O11:O70)</f>
-        <v>0.13975903614457832</v>
+        <v>0.17309236947791165</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
@@ -2903,7 +2906,7 @@
         <v>154</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" ref="O11:O17" si="0">SUM(($J11-$D$1), ($K11-$D$1), ($L11-$D$1), ($M11-$D$1), ($N11-$D$1))/($D$3*5)</f>
+        <f t="shared" ref="O11:O18" si="0">SUM(($J11-$D$1), ($K11-$D$1), ($L11-$D$1), ($M11-$D$1), ($N11-$D$1))/($D$3*5)</f>
         <v>0</v>
       </c>
       <c r="P11" s="4">
@@ -3166,7 +3169,7 @@
         <v>0.12409638554216867</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" ref="P16:P18" si="6">1-O16</f>
+        <f t="shared" ref="P16:P19" si="6">1-O16</f>
         <v>0.87590361445783138</v>
       </c>
     </row>
@@ -3250,8 +3253,29 @@
         <f t="shared" si="2"/>
         <v>0.82128514056224899</v>
       </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="4"/>
+      <c r="J18" s="1">
+        <v>469</v>
+      </c>
+      <c r="K18" s="1">
+        <v>183</v>
+      </c>
+      <c r="L18" s="1">
+        <v>183</v>
+      </c>
+      <c r="M18" s="1">
+        <v>183</v>
+      </c>
+      <c r="N18" s="1">
+        <v>183</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17309236947791165</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="6"/>
+        <v>0.82690763052208838</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B19" s="3">

</xml_diff>